<commit_message>
that should be all the xlsx data we want
</commit_message>
<xml_diff>
--- a/genetic_algorithm_results.xlsx
+++ b/genetic_algorithm_results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,12 +434,42 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Mines</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Missing Mines</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>Fitness</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Max Fitness</t>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t># Flags in solution</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Total mines</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t># Correct Flags</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>% Correctly Identified</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Max Possible Fitness</t>
         </is>
       </c>
     </row>
@@ -451,15 +481,43 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{(4, 4), (3, 8), (2, 2), (6, 5), (4, 6), (4, 2), (1, 7), (5, 6), (3, 6)}</t>
+          <t>{(5, 5), (3, 4), (1, 5), (3, 1), (4, 6), (8, 6), (6, 3), (1, 3), (3, 5)}</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>510</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
+          <t>{(5, 5), (7, 1), (3, 4), (1, 5), (3, 1), (4, 6), (8, 6), (6, 3), (1, 3), (3, 5)}</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>(7, 1)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>516</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>90</v>
+      </c>
+      <c r="J2" t="n">
         <v>571</v>
       </c>
     </row>
@@ -471,15 +529,43 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>{(4, 4), (0, 7), (3, 8), (6, 5), (3, 7), (4, 2), (1, 7), (5, 6), (3, 6)}</t>
+          <t>{(5, 5), (7, 1), (1, 5), (3, 1), (4, 6), (8, 6), (6, 3), (1, 3), (3, 5)}</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>510</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
+          <t>{(5, 5), (7, 1), (3, 4), (1, 5), (3, 1), (4, 6), (8, 6), (6, 3), (1, 3), (3, 5)}</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>(3, 4)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>516</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>90</v>
+      </c>
+      <c r="J3" t="n">
         <v>571</v>
       </c>
     </row>
@@ -491,15 +577,39 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>{(4, 4), (0, 7), (2, 2), (6, 5), (3, 7), (4, 6), (4, 2), (1, 7), (5, 6), (3, 6)}</t>
+          <t>{(5, 5), (7, 1), (3, 4), (1, 5), (3, 1), (4, 6), (8, 6), (6, 3), (1, 3), (3, 5)}</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>565</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+          <t>{(5, 5), (7, 1), (3, 4), (1, 5), (3, 1), (4, 6), (8, 6), (6, 3), (1, 3), (3, 5)}</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>571</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>100</v>
+      </c>
+      <c r="J4" t="n">
         <v>571</v>
       </c>
     </row>
@@ -511,15 +621,43 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>{(4, 4), (0, 7), (3, 8), (2, 2), (6, 5), (3, 7), (4, 6), (1, 7), (5, 6), (3, 6)}</t>
+          <t>{(5, 5), (7, 1), (3, 4), (1, 5), (3, 1), (4, 6), (6, 3), (1, 3), (3, 5)}</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>565</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
+          <t>{(5, 5), (7, 1), (3, 4), (1, 5), (3, 1), (4, 6), (8, 6), (6, 3), (1, 3), (3, 5)}</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>(8, 6)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>516</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>90</v>
+      </c>
+      <c r="J5" t="n">
         <v>571</v>
       </c>
     </row>
@@ -531,15 +669,43 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>{(4, 4), (0, 7), (2, 2), (6, 5), (3, 7), (4, 6), (4, 2), (1, 7), (5, 6), (3, 6)}</t>
+          <t>{(5, 5), (3, 4), (1, 5), (3, 1), (4, 6), (8, 6), (6, 3), (1, 3), (3, 5)}</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>565</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
+          <t>{(5, 5), (7, 1), (3, 4), (1, 5), (3, 1), (4, 6), (8, 6), (6, 3), (1, 3), (3, 5)}</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>(7, 1)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>516</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>90</v>
+      </c>
+      <c r="J6" t="n">
         <v>571</v>
       </c>
     </row>

</xml_diff>